<commit_message>
new christi data binding
</commit_message>
<xml_diff>
--- a/Christi - Data Binding.xlsx
+++ b/Christi - Data Binding.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\git\LearningManagementWeb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1003B111-2135-4719-9E03-965692EED828}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FA4C9E-98C7-45A2-893E-CDBE427EA3F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="7" xr2:uid="{1D0504FE-B408-44BD-A9E7-7F1F2ED7EF33}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="9" xr2:uid="{1D0504FE-B408-44BD-A9E7-7F1F2ED7EF33}"/>
   </bookViews>
   <sheets>
     <sheet name="search" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="69">
   <si>
     <t>search module</t>
   </si>
@@ -212,9 +212,6 @@
     <t>error, expected file csv</t>
   </si>
   <si>
-    <t>Some header missing or invalid</t>
-  </si>
-  <si>
     <t>Success insert Pre-Test/Post-Test</t>
   </si>
   <si>
@@ -246,6 +243,12 @@
   </si>
   <si>
     <t>NEOP SALES</t>
+  </si>
+  <si>
+    <t>file size exceeded limit</t>
+  </si>
+  <si>
+    <t>C:\Users\ASUS\git\LearningManagementWeb\konten lms\big file.csv</t>
   </si>
 </sst>
 </file>
@@ -770,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7F5E2F0-3624-4CCF-9837-1CA71F76DF0D}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,10 +807,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -815,10 +818,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" t="s">
         <v>57</v>
-      </c>
-      <c r="B4" t="s">
-        <v>58</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -1400,7 +1403,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>7</v>
@@ -1430,7 +1433,7 @@
         <v>4</v>
       </c>
       <c r="K2" s="27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1444,7 +1447,7 @@
         <v>28</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
@@ -1461,22 +1464,22 @@
         <v>4</v>
       </c>
       <c r="K3" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="5" t="s">
@@ -1492,12 +1495,12 @@
         <v>4</v>
       </c>
       <c r="K4" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>7</v>
@@ -1508,7 +1511,7 @@
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>9</v>
@@ -1523,12 +1526,12 @@
         <v>4</v>
       </c>
       <c r="K5" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B6" s="22" t="s">
         <v>7</v>
@@ -1554,12 +1557,12 @@
         <v>3</v>
       </c>
       <c r="K6" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>7</v>
@@ -1585,18 +1588,18 @@
         <v>3</v>
       </c>
       <c r="K7" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="16"/>
@@ -1614,18 +1617,18 @@
         <v>3</v>
       </c>
       <c r="K8" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="16" t="s">
@@ -1645,12 +1648,12 @@
         <v>3</v>
       </c>
       <c r="K9" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>7</v>
@@ -1674,12 +1677,12 @@
         <v>3</v>
       </c>
       <c r="K10" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" s="22" t="s">
         <v>7</v>
@@ -1705,7 +1708,7 @@
         <v>3</v>
       </c>
       <c r="K11" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1732,7 +1735,7 @@
         <v>3</v>
       </c>
       <c r="K12" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1749,7 +1752,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC65C5AD-3475-4492-97A7-C04D1EE102F1}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -1768,7 +1771,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -1839,7 +1842,7 @@
         <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Christi update 17 Juni 2020
</commit_message>
<xml_diff>
--- a/Christi - Data Binding.xlsx
+++ b/Christi - Data Binding.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\git\LearningManagementWeb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\git\LearningManagementWebs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD0B0AB-763F-4F1F-B3DA-715EBC4DBC2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B707BE-92E7-41CA-8AC2-BCAA38A5CD7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="717" firstSheet="5" activeTab="11" xr2:uid="{1D0504FE-B408-44BD-A9E7-7F1F2ED7EF33}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="717" firstSheet="10" activeTab="12" xr2:uid="{1D0504FE-B408-44BD-A9E7-7F1F2ED7EF33}"/>
   </bookViews>
   <sheets>
     <sheet name="search" sheetId="1" r:id="rId1"/>
@@ -23,8 +23,11 @@
     <sheet name="delete slider" sheetId="8" r:id="rId8"/>
     <sheet name="upload quiz" sheetId="9" r:id="rId9"/>
     <sheet name="upload pretest-posttest" sheetId="10" r:id="rId10"/>
-    <sheet name="Sheet1" sheetId="12" r:id="rId11"/>
-    <sheet name="delete test" sheetId="13" r:id="rId12"/>
+    <sheet name="User &amp; Admin" sheetId="12" r:id="rId11"/>
+    <sheet name="new module &amp; submodule" sheetId="15" r:id="rId12"/>
+    <sheet name="delete faq" sheetId="17" r:id="rId13"/>
+    <sheet name="edit" sheetId="14" r:id="rId14"/>
+    <sheet name="edit  module" sheetId="16" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="204">
   <si>
     <t>search module</t>
   </si>
@@ -370,20 +373,299 @@
     <t>1m 7s</t>
   </si>
   <si>
-    <t>searchID</t>
-  </si>
-  <si>
-    <t>keterangan</t>
-  </si>
-  <si>
-    <t>kondisi</t>
+    <t>learning_code</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>course_name</t>
+  </si>
+  <si>
+    <t>module_category</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>tags</t>
+  </si>
+  <si>
+    <t>prerequisite</t>
+  </si>
+  <si>
+    <t>img_upload</t>
+  </si>
+  <si>
+    <t>expected_img_upload</t>
+  </si>
+  <si>
+    <t>New Module</t>
+  </si>
+  <si>
+    <t>Basic Training</t>
+  </si>
+  <si>
+    <t>C:\Users\ASUS\Pictures\Content LMS\PNG_GENERAL Icon.png</t>
+  </si>
+  <si>
+    <t>success</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>search_by</t>
+  </si>
+  <si>
+    <t>type_search</t>
+  </si>
+  <si>
+    <t>expected_search</t>
+  </si>
+  <si>
+    <t>empty</t>
+  </si>
+  <si>
+    <t>Level 2 - Coordinator Training</t>
+  </si>
+  <si>
+    <t>training</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>Module 061520201</t>
+  </si>
+  <si>
+    <t>Module 061520202</t>
+  </si>
+  <si>
+    <t>lorem ipsum</t>
+  </si>
+  <si>
+    <t>Module 061520203</t>
+  </si>
+  <si>
+    <t>submodule_name</t>
+  </si>
+  <si>
+    <t>create_module_expected</t>
+  </si>
+  <si>
+    <t>section_name</t>
+  </si>
+  <si>
+    <t>section_order</t>
+  </si>
+  <si>
+    <t>section_time</t>
+  </si>
+  <si>
+    <t>create_submodule_expected</t>
+  </si>
+  <si>
+    <t>section one</t>
+  </si>
+  <si>
+    <t>section two</t>
+  </si>
+  <si>
+    <t>PDF</t>
+  </si>
+  <si>
+    <t>Video</t>
+  </si>
+  <si>
+    <t>Submodule</t>
+  </si>
+  <si>
+    <t>Submodule 061520202</t>
+  </si>
+  <si>
+    <t>section_file_upload</t>
+  </si>
+  <si>
+    <t>C:\Users\ASUS\git\LearningManagementWeb\konten lms\01. Lemon Rules.pdf</t>
+  </si>
+  <si>
+    <t>‪C:\Users\ASUS\git\LearningManagementWeb\konten lms\01. Pengantar Basic Training.mp4</t>
+  </si>
+  <si>
+    <t>Module 061520204</t>
+  </si>
+  <si>
+    <t>search_module</t>
+  </si>
+  <si>
+    <t>module name</t>
+  </si>
+  <si>
+    <t>learning code</t>
+  </si>
+  <si>
+    <t>course name</t>
+  </si>
+  <si>
+    <t>module category</t>
+  </si>
+  <si>
+    <t>img</t>
+  </si>
+  <si>
+    <t>submodule name</t>
+  </si>
+  <si>
+    <t>section name</t>
+  </si>
+  <si>
+    <t>section order</t>
+  </si>
+  <si>
+    <t>section time</t>
+  </si>
+  <si>
+    <t>SALES HEAD</t>
+  </si>
+  <si>
+    <t>Coordinator up</t>
+  </si>
+  <si>
+    <t>edit desc</t>
+  </si>
+  <si>
+    <t>sales</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>section_format</t>
+  </si>
+  <si>
+    <t>section format</t>
+  </si>
+  <si>
+    <t>Sub module xx</t>
+  </si>
+  <si>
+    <t>section xx</t>
+  </si>
+  <si>
+    <t>‪C:\Users\ASUS\git\LearningManagementWeb\konten lms\PNG_UW Icon .png</t>
+  </si>
+  <si>
+    <t>Level 3 - Head Training</t>
+  </si>
+  <si>
+    <t>Level 4 - Branch Manager Training</t>
+  </si>
+  <si>
+    <t>Level 5 - Division Training</t>
+  </si>
+  <si>
+    <t>Level 6 - Regional Training</t>
+  </si>
+  <si>
+    <t>Level 7 - Chief Training</t>
+  </si>
+  <si>
+    <t>Level 8 - CEO Training</t>
+  </si>
+  <si>
+    <t>BRANCH UNDERWRITING HEAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AR MANAGEMENT HEAD </t>
+  </si>
+  <si>
+    <t>SERVICE HEAD</t>
+  </si>
+  <si>
+    <t>DESKCOLL COORDINATOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RECOVERY MANAGEMENT HEAD </t>
+  </si>
+  <si>
+    <t>FINANCE &amp; BANKING OFFICER</t>
+  </si>
+  <si>
+    <t>OPERATION HEAD</t>
+  </si>
+  <si>
+    <t>CUSTOMER SERVICE OFFICER</t>
+  </si>
+  <si>
+    <t>SURVEYOR HEAD</t>
+  </si>
+  <si>
+    <t>New Employee Orientation Program</t>
+  </si>
+  <si>
+    <t>General Knowledge</t>
+  </si>
+  <si>
+    <t>Inactive</t>
+  </si>
+  <si>
+    <t>New Module X</t>
+  </si>
+  <si>
+    <t>VIDEO</t>
+  </si>
+  <si>
+    <t>QUIZ</t>
+  </si>
+  <si>
+    <t>Submodule 061520203</t>
+  </si>
+  <si>
+    <t>Submodule 061520204</t>
+  </si>
+  <si>
+    <t>section three</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>general</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>new_submodule</t>
+  </si>
+  <si>
+    <t>var_search</t>
+  </si>
+  <si>
+    <t>expected_delete</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>question14</t>
+  </si>
+  <si>
+    <t>answer14</t>
+  </si>
+  <si>
+    <t>cancel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -416,6 +698,12 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -498,7 +786,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -537,6 +825,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -988,7 +1285,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1044,674 +1341,1414 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F20AF2B-39BE-4463-B573-4D2A75D5EAFA}">
-  <dimension ref="A1:C82"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BAF8056-653C-4054-B3C3-E497E037C383}">
+  <dimension ref="A1:W13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B20" activeCellId="1" sqref="B31:B82 B20:B29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="57.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" customWidth="1"/>
+    <col min="13" max="13" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>123</v>
+      </c>
+      <c r="C2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E2" t="s">
+        <v>185</v>
+      </c>
+      <c r="F2" t="s">
+        <v>132</v>
+      </c>
+      <c r="I2" t="s">
+        <v>121</v>
+      </c>
+      <c r="J2" t="s">
+        <v>119</v>
+      </c>
+      <c r="K2" t="s">
+        <v>120</v>
+      </c>
+      <c r="L2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D3" t="s">
+        <v>160</v>
+      </c>
+      <c r="E3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F3" t="s">
+        <v>132</v>
+      </c>
+      <c r="I3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J3" t="s">
+        <v>119</v>
+      </c>
+      <c r="K3" t="s">
+        <v>120</v>
+      </c>
+      <c r="L3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4">
+        <v>123</v>
+      </c>
+      <c r="D4" t="s">
+        <v>176</v>
+      </c>
+      <c r="E4" t="s">
+        <v>186</v>
+      </c>
+      <c r="F4" t="s">
+        <v>132</v>
+      </c>
+      <c r="I4" t="s">
+        <v>121</v>
+      </c>
+      <c r="J4" t="s">
+        <v>119</v>
+      </c>
+      <c r="K4" t="s">
+        <v>120</v>
+      </c>
+      <c r="L4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5">
+        <v>123</v>
+      </c>
+      <c r="C5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F5" t="s">
+        <v>132</v>
+      </c>
+      <c r="I5" t="s">
+        <v>187</v>
+      </c>
+      <c r="J5" t="s">
+        <v>119</v>
+      </c>
+      <c r="K5" t="s">
+        <v>120</v>
+      </c>
+      <c r="L5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6">
+        <v>123</v>
+      </c>
+      <c r="C6" t="s">
+        <v>172</v>
+      </c>
+      <c r="D6" t="s">
+        <v>177</v>
+      </c>
+      <c r="F6" t="s">
+        <v>132</v>
+      </c>
+      <c r="I6" t="s">
+        <v>121</v>
+      </c>
+      <c r="J6" t="s">
+        <v>119</v>
+      </c>
+      <c r="K6" t="s">
+        <v>120</v>
+      </c>
+      <c r="L6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7">
+        <v>123</v>
+      </c>
+      <c r="C7" t="s">
+        <v>173</v>
+      </c>
+      <c r="D7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E7" t="s">
+        <v>185</v>
+      </c>
+      <c r="I7" t="s">
+        <v>187</v>
+      </c>
+      <c r="J7" t="s">
+        <v>119</v>
+      </c>
+      <c r="K7" t="s">
+        <v>120</v>
+      </c>
+      <c r="L7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B8">
+        <v>123</v>
+      </c>
+      <c r="C8" t="s">
+        <v>174</v>
+      </c>
+      <c r="D8" t="s">
+        <v>179</v>
+      </c>
+      <c r="E8" t="s">
+        <v>118</v>
+      </c>
+      <c r="F8" t="s">
+        <v>132</v>
+      </c>
+      <c r="J8" t="s">
+        <v>119</v>
+      </c>
+      <c r="K8" t="s">
+        <v>120</v>
+      </c>
+      <c r="L8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B9">
+        <v>123</v>
+      </c>
+      <c r="C9" t="s">
+        <v>175</v>
+      </c>
+      <c r="D9" t="s">
+        <v>180</v>
+      </c>
+      <c r="E9" t="s">
+        <v>186</v>
+      </c>
+      <c r="F9" t="s">
+        <v>132</v>
+      </c>
+      <c r="I9" t="s">
+        <v>121</v>
+      </c>
+      <c r="K9" t="s">
+        <v>125</v>
+      </c>
+      <c r="L9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B10">
+        <v>123</v>
+      </c>
+      <c r="C10" t="s">
+        <v>126</v>
+      </c>
+      <c r="D10" t="s">
+        <v>181</v>
+      </c>
+      <c r="E10" t="s">
+        <v>161</v>
+      </c>
+      <c r="F10" t="s">
+        <v>127</v>
+      </c>
+      <c r="I10" t="s">
+        <v>187</v>
+      </c>
+      <c r="J10" t="s">
+        <v>119</v>
+      </c>
+      <c r="K10" t="s">
+        <v>120</v>
+      </c>
+      <c r="L10" t="s">
+        <v>4</v>
+      </c>
+      <c r="M10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B11">
+        <v>123</v>
+      </c>
+      <c r="C11" t="s">
+        <v>170</v>
+      </c>
+      <c r="D11" t="s">
+        <v>182</v>
+      </c>
+      <c r="E11" t="s">
+        <v>185</v>
+      </c>
+      <c r="F11" t="s">
+        <v>127</v>
+      </c>
+      <c r="G11" t="s">
+        <v>182</v>
+      </c>
+      <c r="I11" t="s">
+        <v>121</v>
+      </c>
+      <c r="J11" t="s">
+        <v>119</v>
+      </c>
+      <c r="K11" t="s">
+        <v>120</v>
+      </c>
+      <c r="L11" t="s">
+        <v>4</v>
+      </c>
+      <c r="M11" t="s">
+        <v>11</v>
+      </c>
+      <c r="N11" t="s">
+        <v>145</v>
+      </c>
+      <c r="O11" t="s">
+        <v>140</v>
+      </c>
+      <c r="P11" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>147</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+      <c r="S11">
+        <v>300</v>
+      </c>
+      <c r="T11" t="s">
+        <v>4</v>
+      </c>
+      <c r="U11" t="s">
+        <v>144</v>
+      </c>
+      <c r="V11" t="s">
+        <v>145</v>
+      </c>
+      <c r="W11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>133</v>
+      </c>
+      <c r="B12">
+        <v>123</v>
+      </c>
+      <c r="C12" t="s">
+        <v>171</v>
+      </c>
+      <c r="D12" t="s">
+        <v>183</v>
+      </c>
+      <c r="E12" t="s">
+        <v>118</v>
+      </c>
+      <c r="F12" t="s">
+        <v>127</v>
+      </c>
+      <c r="G12" t="s">
+        <v>183</v>
+      </c>
+      <c r="H12" t="s">
+        <v>128</v>
+      </c>
+      <c r="I12" t="s">
+        <v>121</v>
+      </c>
+      <c r="J12" t="s">
+        <v>119</v>
+      </c>
+      <c r="K12" t="s">
+        <v>120</v>
+      </c>
+      <c r="L12" t="s">
+        <v>4</v>
+      </c>
+      <c r="M12" t="s">
+        <v>11</v>
+      </c>
+      <c r="N12" t="s">
+        <v>191</v>
+      </c>
+      <c r="O12" t="s">
+        <v>141</v>
+      </c>
+      <c r="P12" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>148</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>690</v>
+      </c>
+      <c r="T12" t="s">
+        <v>3</v>
+      </c>
+      <c r="U12" t="s">
+        <v>129</v>
+      </c>
+      <c r="V12" t="s">
+        <v>133</v>
+      </c>
+      <c r="W12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>149</v>
+      </c>
+      <c r="B13">
+        <v>123</v>
+      </c>
+      <c r="C13" t="s">
+        <v>172</v>
+      </c>
+      <c r="D13" t="s">
+        <v>184</v>
+      </c>
+      <c r="E13" t="s">
+        <v>186</v>
+      </c>
+      <c r="F13" t="s">
+        <v>127</v>
+      </c>
+      <c r="G13" t="s">
+        <v>184</v>
+      </c>
+      <c r="H13" t="s">
+        <v>128</v>
+      </c>
+      <c r="I13" t="s">
+        <v>121</v>
+      </c>
+      <c r="J13" t="s">
+        <v>119</v>
+      </c>
+      <c r="K13" t="s">
+        <v>120</v>
+      </c>
+      <c r="L13" t="s">
+        <v>4</v>
+      </c>
+      <c r="M13" t="s">
+        <v>11</v>
+      </c>
+      <c r="N13" t="s">
+        <v>192</v>
+      </c>
+      <c r="O13" t="s">
+        <v>193</v>
+      </c>
+      <c r="P13" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>148</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+      <c r="S13">
+        <v>690</v>
+      </c>
+      <c r="T13" t="s">
+        <v>3</v>
+      </c>
+      <c r="U13" t="s">
+        <v>129</v>
+      </c>
+      <c r="V13" t="s">
+        <v>133</v>
+      </c>
+      <c r="W13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6EF164D-8FEA-4049-BFB2-F4BD44E61E80}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>201</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE83CA42-3BCF-43C6-8CB3-3565ACEF695D}">
+  <dimension ref="A1:U17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="G1" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="I1" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="K1" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="L1" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="N1" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="O1" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="P1" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q1" s="31" t="s">
+        <v>165</v>
+      </c>
+      <c r="R1" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="S1" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="T1" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="U1" s="31" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D3" t="s">
+        <v>188</v>
+      </c>
+      <c r="U3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E4">
+        <v>101</v>
+      </c>
+      <c r="U4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1755</v>
+      <c r="F5" t="s">
+        <v>170</v>
+      </c>
+      <c r="U5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>188</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G6" t="s">
+        <v>160</v>
+      </c>
+      <c r="U6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>188</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>154</v>
+      </c>
+      <c r="H7" t="s">
+        <v>161</v>
+      </c>
+      <c r="U7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>188</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>112</v>
+      </c>
+      <c r="I8" t="s">
+        <v>162</v>
+      </c>
+      <c r="U8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>188</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>113</v>
+      </c>
+      <c r="J9" t="s">
+        <v>163</v>
+      </c>
+      <c r="U9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>188</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>114</v>
+      </c>
+      <c r="K10" t="s">
+        <v>164</v>
+      </c>
+      <c r="U10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>188</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="L11" t="s">
+        <v>121</v>
+      </c>
+      <c r="U11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>188</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>155</v>
+      </c>
+      <c r="M12" t="s">
+        <v>169</v>
+      </c>
+      <c r="N12" t="s">
+        <v>4</v>
+      </c>
+      <c r="U12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>186</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="33"/>
+      <c r="L13" s="33"/>
+      <c r="M13" s="33"/>
+      <c r="N13" s="33"/>
+      <c r="O13" s="34" t="s">
+        <v>167</v>
+      </c>
+      <c r="P13" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q13" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="R13" s="34"/>
+      <c r="S13" s="34">
+        <v>1</v>
+      </c>
+      <c r="T13" s="34">
+        <v>180</v>
+      </c>
+      <c r="U13" s="34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>188</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>157</v>
+      </c>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q14" s="30"/>
+      <c r="R14" s="30"/>
+      <c r="S14" s="30"/>
+      <c r="T14" s="30"/>
+      <c r="U14" s="30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>188</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="30"/>
+      <c r="P15" s="30"/>
+      <c r="Q15" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="R15" s="30"/>
+      <c r="S15" s="30"/>
+      <c r="T15" s="30"/>
+      <c r="U15" s="30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>188</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="30"/>
+      <c r="P16" s="30"/>
+      <c r="Q16" s="30"/>
+      <c r="R16" s="30"/>
+      <c r="S16" s="30">
+        <v>2</v>
+      </c>
+      <c r="T16" s="30"/>
+      <c r="U16" s="30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>188</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>159</v>
+      </c>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="30"/>
+      <c r="O17" s="30"/>
+      <c r="P17" s="30"/>
+      <c r="Q17" s="30"/>
+      <c r="R17" s="30"/>
+      <c r="S17" s="30"/>
+      <c r="T17" s="30">
+        <v>600</v>
+      </c>
+      <c r="U17" s="30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C4B7E34-FBD6-4990-B585-5AF3A2550AC8}">
+  <dimension ref="A1:O13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" customWidth="1"/>
+    <col min="14" max="14" width="21" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="H1" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="I1" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="K1" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="L1" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="N1" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="O1" s="31" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1756</v>
+        <v>38</v>
+      </c>
+      <c r="O2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>117</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1757</v>
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D3" t="s">
+        <v>188</v>
+      </c>
+      <c r="O3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>188</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1758</v>
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E4">
+        <v>101</v>
+      </c>
+      <c r="O4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>188</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1759</v>
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F5" t="s">
+        <v>170</v>
+      </c>
+      <c r="O5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>188</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1760</v>
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G6" t="s">
+        <v>160</v>
+      </c>
+      <c r="O6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>188</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1761</v>
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>154</v>
+      </c>
+      <c r="H7" t="s">
+        <v>161</v>
+      </c>
+      <c r="O7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>188</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1762</v>
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>112</v>
+      </c>
+      <c r="I8" t="s">
+        <v>162</v>
+      </c>
+      <c r="O8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>188</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1763</v>
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>113</v>
+      </c>
+      <c r="J9" t="s">
+        <v>163</v>
+      </c>
+      <c r="O9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>188</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1764</v>
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>114</v>
+      </c>
+      <c r="K10" t="s">
+        <v>164</v>
+      </c>
+      <c r="O10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>188</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1765</v>
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="L11" t="s">
+        <v>121</v>
+      </c>
+      <c r="O11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>188</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>1766</v>
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>155</v>
+      </c>
+      <c r="M12" t="s">
+        <v>169</v>
+      </c>
+      <c r="N12" t="s">
+        <v>4</v>
+      </c>
+      <c r="O12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>188</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>1767</v>
-      </c>
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>1768</v>
-      </c>
-      <c r="B15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>1769</v>
-      </c>
-      <c r="B16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>1770</v>
-      </c>
-      <c r="B17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>1771</v>
-      </c>
-      <c r="B18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>1772</v>
-      </c>
-      <c r="B19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>1773</v>
-      </c>
-      <c r="B20" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>1774</v>
-      </c>
-      <c r="B21" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>1775</v>
-      </c>
-      <c r="B22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>1776</v>
-      </c>
-      <c r="B23" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>1777</v>
-      </c>
-      <c r="B24" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>1778</v>
-      </c>
-      <c r="B25" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>1779</v>
-      </c>
-      <c r="B26" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>1780</v>
-      </c>
-      <c r="B27" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>1781</v>
-      </c>
-      <c r="B28" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>1782</v>
-      </c>
-      <c r="B29" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>1783</v>
-      </c>
-      <c r="B30" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>1784</v>
-      </c>
-      <c r="B31" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>1785</v>
-      </c>
-      <c r="B32" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>1786</v>
-      </c>
-      <c r="B33" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>1787</v>
-      </c>
-      <c r="B34" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>1788</v>
-      </c>
-      <c r="B35" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>1789</v>
-      </c>
-      <c r="B36" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>1790</v>
-      </c>
-      <c r="B37" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>1791</v>
-      </c>
-      <c r="B38" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>1792</v>
-      </c>
-      <c r="B39" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>1793</v>
-      </c>
-      <c r="B40" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>1794</v>
-      </c>
-      <c r="B41" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>1795</v>
-      </c>
-      <c r="B42" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>1796</v>
-      </c>
-      <c r="B43" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>1797</v>
-      </c>
-      <c r="B44" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>1798</v>
-      </c>
-      <c r="B45" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>1799</v>
-      </c>
-      <c r="B46" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>1800</v>
-      </c>
-      <c r="B47" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>1801</v>
-      </c>
-      <c r="B48" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>1802</v>
-      </c>
-      <c r="B49" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>1803</v>
-      </c>
-      <c r="B50" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>1804</v>
-      </c>
-      <c r="B51" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>1805</v>
-      </c>
-      <c r="B52" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>1806</v>
-      </c>
-      <c r="B53" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>1807</v>
-      </c>
-      <c r="B54" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>1808</v>
-      </c>
-      <c r="B55" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>1809</v>
-      </c>
-      <c r="B56" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>1810</v>
-      </c>
-      <c r="B57" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>1811</v>
-      </c>
-      <c r="B58" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>1812</v>
-      </c>
-      <c r="B59" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>1813</v>
-      </c>
-      <c r="B60" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>1814</v>
-      </c>
-      <c r="B61" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>1815</v>
-      </c>
-      <c r="B62" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>1816</v>
-      </c>
-      <c r="B63" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>1817</v>
-      </c>
-      <c r="B64" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>1818</v>
-      </c>
-      <c r="B65" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>1819</v>
-      </c>
-      <c r="B66" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <v>1820</v>
-      </c>
-      <c r="B67" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <v>1821</v>
-      </c>
-      <c r="B68" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69">
-        <v>1822</v>
-      </c>
-      <c r="B69" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <v>1823</v>
-      </c>
-      <c r="B70" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71">
-        <v>1824</v>
-      </c>
-      <c r="B71" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <v>1825</v>
-      </c>
-      <c r="B72" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <v>1826</v>
-      </c>
-      <c r="B73" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <v>1827</v>
-      </c>
-      <c r="B74" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>1828</v>
-      </c>
-      <c r="B75" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <v>1829</v>
-      </c>
-      <c r="B76" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <v>1830</v>
-      </c>
-      <c r="B77" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78">
-        <v>1831</v>
-      </c>
-      <c r="B78" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79">
-        <v>1832</v>
-      </c>
-      <c r="B79" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80">
-        <v>1833</v>
-      </c>
-      <c r="B80" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81">
-        <v>1834</v>
-      </c>
-      <c r="B81" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82">
-        <v>1835</v>
-      </c>
-      <c r="B82" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>194</v>
+      </c>
+      <c r="D13" t="s">
+        <v>186</v>
+      </c>
+      <c r="E13">
+        <v>111</v>
+      </c>
+      <c r="F13" t="s">
+        <v>171</v>
+      </c>
+      <c r="G13" t="s">
+        <v>183</v>
+      </c>
+      <c r="H13" t="s">
+        <v>186</v>
+      </c>
+      <c r="I13" t="s">
+        <v>132</v>
+      </c>
+      <c r="J13" t="s">
+        <v>195</v>
+      </c>
+      <c r="K13" t="s">
+        <v>196</v>
+      </c>
+      <c r="L13" t="s">
+        <v>121</v>
+      </c>
+      <c r="M13" t="s">
+        <v>119</v>
+      </c>
+      <c r="N13" t="s">
+        <v>4</v>
+      </c>
+      <c r="O13" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>